<commit_message>
Added new quenching plots. Updated several plots for publication
</commit_message>
<xml_diff>
--- a/AdditionalData/LumFunc.xlsx
+++ b/AdditionalData/LumFunc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdvannest/Pynbody/SAGA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdvannest/Pynbody/MilkyWayAnalogs/AdditionalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD49377E-ABE6-A54C-8C2B-41510A33F407}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A6E710-640F-3C49-90E6-E52422DFCA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{8F2EF17A-7CC1-7F40-8CBF-12BD1FB2A0CD}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16060" xr2:uid="{8F2EF17A-7CC1-7F40-8CBF-12BD1FB2A0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,19 +31,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>MW</t>
   </si>
   <si>
     <t>M31</t>
   </si>
+  <si>
+    <t>M101</t>
+  </si>
+  <si>
+    <t>M94</t>
+  </si>
+  <si>
+    <t>Cen A</t>
+  </si>
+  <si>
+    <t>M81</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -389,13 +407,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B602CC-14B4-C346-9CE4-14547158A37D}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
@@ -403,15 +421,27 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>-18.303217131103501</v>
       </c>
@@ -424,8 +454,32 @@
       <c r="D2" s="1">
         <v>7.1857942375430596E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>-18.303217131103501</v>
       </c>
@@ -438,8 +492,32 @@
       <c r="D3" s="1">
         <v>7.1857942375430596E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="1">
+        <v>-20.812807881773399</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.01664096207925</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-19.605911330049199</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.0068687387412001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-21.009852216748701</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.0104288647293</v>
+      </c>
+      <c r="K3" s="1">
+        <v>-20.209359605911299</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.00705681083056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>-18.302171151587299</v>
       </c>
@@ -452,8 +530,32 @@
       <c r="D4" s="1">
         <v>1.0074866196471901</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1">
+        <v>-17.610837438423601</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.0065744713948099</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-14.310344827586199</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.0045257489352801</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-17.413793103448199</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2.0002515857879901</v>
+      </c>
+      <c r="K4" s="1">
+        <v>-19.519704433497498</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2.0077603224220399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>-17.001304285433299</v>
       </c>
@@ -466,8 +568,32 @@
       <c r="D5" s="1">
         <v>1.00402340698063</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1">
+        <v>-15.295566502463</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.01699727149636</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-10.615763546798</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3.0126305159217099</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-15.7635467980295</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3.0174342950270501</v>
+      </c>
+      <c r="K5" s="1">
+        <v>-17.598522167487602</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3.0005172532380202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>-17.0002583059171</v>
       </c>
@@ -480,8 +606,32 @@
       <c r="D6" s="1">
         <v>2.0026723501055002</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="1">
+        <v>-15</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.0354080700646202</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-10.0985221674876</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4.0044259634478703</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-15.246305418719199</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4.02324419007748</v>
+      </c>
+      <c r="K6" s="1">
+        <v>-17.413793103448199</v>
+      </c>
+      <c r="L6" s="1">
+        <v>4.00109989492484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>-13.7009582830628</v>
       </c>
@@ -494,8 +644,32 @@
       <c r="D7" s="1">
         <v>2.0028891995174001</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="1">
+        <v>-9.5812807881773399</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5.0343053153774902</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-9.7044334975369395</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5.0501034846892301</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-14.113300492610801</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5.0413718558473901</v>
+      </c>
+      <c r="K7" s="1">
+        <v>-17.315270935960498</v>
+      </c>
+      <c r="L7" s="1">
+        <v>5.01522921396844</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>-13.6999208074451</v>
       </c>
@@ -508,8 +682,26 @@
       <c r="D8" s="1">
         <v>3.0015381426422598</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="1">
+        <v>-9.5073891625615694</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6.02409285299583</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-13.842364532019699</v>
+      </c>
+      <c r="J8" s="1">
+        <v>6.0508798039699601</v>
+      </c>
+      <c r="K8" s="1">
+        <v>-14.6921182266009</v>
+      </c>
+      <c r="L8" s="1">
+        <v>6.0151214641302504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>-13.599370711510501</v>
       </c>
@@ -522,8 +714,26 @@
       <c r="D9" s="1">
         <v>3.00438269669251</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="1">
+        <v>-9.4088669950738897</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7.0104015608791004</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-13.0911330049261</v>
+      </c>
+      <c r="J9" s="1">
+        <v>7.04015188489974</v>
+      </c>
+      <c r="K9" s="1">
+        <v>-14.2118226600985</v>
+      </c>
+      <c r="L9" s="1">
+        <v>7.0208306216276002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>-13.6046091129902</v>
       </c>
@@ -536,8 +746,26 @@
       <c r="D10" s="1">
         <v>4.0030188839696201</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="1">
+        <v>-8.7931034482758594</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8.0565278913005702</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-12.561576354679801</v>
+      </c>
+      <c r="J10" s="1">
+        <v>8.0659302647038498</v>
+      </c>
+      <c r="K10" s="1">
+        <v>-13.201970443349699</v>
+      </c>
+      <c r="L10" s="1">
+        <v>8.0177442092736406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>-12.1969077699057</v>
       </c>
@@ -550,8 +778,26 @@
       <c r="D11" s="1">
         <v>4.0034270710979003</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="1">
+        <v>-8.1034482758620694</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9.0601166768180299</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-12.475369458128</v>
+      </c>
+      <c r="J11" s="1">
+        <v>9.0723845947580806</v>
+      </c>
+      <c r="K11" s="1">
+        <v>-12.906403940886699</v>
+      </c>
+      <c r="L11" s="1">
+        <v>9.0176016132911094</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>-12.195853286490999</v>
       </c>
@@ -564,8 +810,20 @@
       <c r="D12" s="1">
         <v>5.0020760142227703</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="I12" s="1">
+        <v>-12.3522167487684</v>
+      </c>
+      <c r="J12" s="1">
+        <v>10.047606319868001</v>
+      </c>
+      <c r="K12" s="1">
+        <v>-12.807881773399</v>
+      </c>
+      <c r="L12" s="1">
+        <v>10.017969072600399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>-11.297195307974</v>
       </c>
@@ -578,8 +836,20 @@
       <c r="D13" s="1">
         <v>5.0024842013510504</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="I13" s="1">
+        <v>-12.032019704433401</v>
+      </c>
+      <c r="J13" s="1">
+        <v>11.0583144711867</v>
+      </c>
+      <c r="K13" s="1">
+        <v>-12.807881773399</v>
+      </c>
+      <c r="L13" s="1">
+        <v>11.026788693117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>-11.2961493284577</v>
       </c>
@@ -592,8 +862,20 @@
       <c r="D14" s="1">
         <v>6.0011331444759204</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="I14" s="1">
+        <v>-11.933497536945801</v>
+      </c>
+      <c r="J14" s="1">
+        <v>12.0217686561185</v>
+      </c>
+      <c r="K14" s="1">
+        <v>-12.807881773399</v>
+      </c>
+      <c r="L14" s="1">
+        <v>12.025022527161999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>-10.994499040653899</v>
       </c>
@@ -606,69 +888,281 @@
       <c r="D15" s="1">
         <v>6.0051895040632699</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="I15" s="1">
+        <v>-11.182266009852199</v>
+      </c>
+      <c r="J15" s="1">
+        <v>13.026144392932901</v>
+      </c>
+      <c r="K15" s="1">
+        <v>-12.5985221674876</v>
+      </c>
+      <c r="L15" s="1">
+        <v>13.0318555456191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C16" s="1">
         <v>-12.797061903066099</v>
       </c>
       <c r="D16" s="1">
         <v>7.0038384471881301</v>
       </c>
-    </row>
-    <row r="17" spans="3:4">
+      <c r="I16" s="1">
+        <v>-10.8128078817734</v>
+      </c>
+      <c r="J16" s="1">
+        <v>14.01</v>
+      </c>
+      <c r="K16" s="1">
+        <v>-12.586206896551699</v>
+      </c>
+      <c r="L16" s="1">
+        <v>14.0366915295666</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
         <v>-12.5959617111969</v>
       </c>
       <c r="D17" s="1">
         <v>7.00424663431642</v>
       </c>
-    </row>
-    <row r="18" spans="3:4">
+      <c r="I17" s="1">
+        <v>-10.6527093596059</v>
+      </c>
+      <c r="J17" s="1">
+        <v>15.0167748141362</v>
+      </c>
+      <c r="K17" s="1">
+        <v>-12.401477832512301</v>
+      </c>
+      <c r="L17" s="1">
+        <v>15.0249049425449</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
         <v>-12.5949157316807</v>
       </c>
       <c r="D18" s="1">
         <v>8.0028955774412793</v>
       </c>
-    </row>
-    <row r="19" spans="3:4">
+      <c r="I18" s="1">
+        <v>-10.061576354679801</v>
+      </c>
+      <c r="J18" s="1">
+        <v>16.022299462002799</v>
+      </c>
+      <c r="K18" s="1">
+        <v>-12.0197044334975</v>
+      </c>
+      <c r="L18" s="1">
+        <v>16.0320127984808</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <v>-12.494365635746099</v>
       </c>
       <c r="D19" s="1">
         <v>8.0030996710054207</v>
       </c>
-    </row>
-    <row r="20" spans="3:4">
+      <c r="I19" s="1">
+        <v>-9.9014778325123096</v>
+      </c>
+      <c r="J19" s="1">
+        <v>17.010000000000002</v>
+      </c>
+      <c r="K19" s="1">
+        <v>-12.0197044334975</v>
+      </c>
+      <c r="L19" s="1">
+        <v>17.003069872224799</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C20" s="1">
         <v>-12.4933196562299</v>
       </c>
       <c r="D20" s="1">
         <v>9.0017486141302907</v>
       </c>
-    </row>
-    <row r="21" spans="3:4">
+      <c r="I20" s="1">
+        <v>-9.9014778325123096</v>
+      </c>
+      <c r="J20" s="1">
+        <v>18.021125113421501</v>
+      </c>
+      <c r="K20" s="1">
+        <v>-12.0197044334975</v>
+      </c>
+      <c r="L20" s="1">
+        <v>18.032943755331399</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C21" s="1">
         <v>-11.8963034616181</v>
       </c>
       <c r="D21" s="1">
         <v>9.0029604196673905</v>
       </c>
-    </row>
-    <row r="22" spans="3:4">
+      <c r="I21" s="1">
+        <v>-9.7290640394088594</v>
+      </c>
+      <c r="J21" s="1">
+        <v>19.0525821093504</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-11.6995073891625</v>
+      </c>
+      <c r="L21" s="1">
+        <v>19.005291299823298</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C22" s="1">
         <v>-11.895257482101901</v>
       </c>
       <c r="D22" s="1">
         <v>10.0016093627922</v>
       </c>
-    </row>
-    <row r="23" spans="3:4">
+      <c r="I22" s="1">
+        <v>-9.7044334975369395</v>
+      </c>
+      <c r="J22" s="1">
+        <v>20.0196878005938</v>
+      </c>
+      <c r="K22" s="1">
+        <v>-11.317733990147699</v>
+      </c>
+      <c r="L22" s="1">
+        <v>20.029686692721999</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C23" s="1">
         <v>-10.9903066186905</v>
       </c>
       <c r="D23" s="1">
         <v>10.003446204869499</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-9.3965517241379306</v>
+      </c>
+      <c r="J23" s="1">
+        <v>21.034039505560699</v>
+      </c>
+      <c r="K23" s="1">
+        <v>-11.317733990147699</v>
+      </c>
+      <c r="L23" s="1">
+        <v>21.046550483684602</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="I24" s="1">
+        <v>-9.1256157635468007</v>
+      </c>
+      <c r="J24" s="1">
+        <v>22.0317433123661</v>
+      </c>
+      <c r="K24" s="1">
+        <v>-11.317733990147699</v>
+      </c>
+      <c r="L24" s="1">
+        <v>22.046696406166198</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="I25" s="1">
+        <v>-9.1009852216748701</v>
+      </c>
+      <c r="J25" s="1">
+        <v>23.0785303101074</v>
+      </c>
+      <c r="K25" s="1">
+        <v>-9.3842364532019698</v>
+      </c>
+      <c r="L25" s="1">
+        <v>23.080553654808099</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="I26" s="1">
+        <v>-8.2512315270935908</v>
+      </c>
+      <c r="J26" s="1">
+        <v>24.0197330848987</v>
+      </c>
+      <c r="K26" s="1">
+        <v>-9.3842364532019698</v>
+      </c>
+      <c r="L26" s="1">
+        <v>24.0281576406563</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="I27" s="1">
+        <v>-7.8078817733990098</v>
+      </c>
+      <c r="J27" s="1">
+        <v>25.002465305276498</v>
+      </c>
+      <c r="K27" s="1">
+        <v>-9.3842364532019698</v>
+      </c>
+      <c r="L27" s="1">
+        <v>25.014666816017002</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="K28" s="1">
+        <v>-9.0147783251231495</v>
+      </c>
+      <c r="L28" s="1">
+        <v>26.038700791869001</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="K29" s="1">
+        <v>-9.0147783251231495</v>
+      </c>
+      <c r="L29" s="1">
+        <v>27.023984816494099</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="K30" s="1">
+        <v>-9.0147783251231495</v>
+      </c>
+      <c r="L30" s="1">
+        <v>28.046551216186199</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="K31" s="1">
+        <v>-8.9039408866995</v>
+      </c>
+      <c r="L31" s="1">
+        <v>29.016863764999702</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="K32" s="1">
+        <v>-8.3990147783251192</v>
+      </c>
+      <c r="L32" s="1">
+        <v>30.017084226664299</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K33" s="1">
+        <v>-7.9310344827586201</v>
+      </c>
+      <c r="L33" s="1">
+        <v>31.052137682771001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>